<commit_message>
lecture registry and schedule
</commit_message>
<xml_diff>
--- a/project-evaluation.xlsx
+++ b/project-evaluation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Burak\Desktop\Database Systems\SchoolManager\itucsdb1932\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furka\Desktop\dersler\database\gitproje\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BC7B9C-E904-423D-88D9-0F89DF85A678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F416ECF-9B06-4AF7-81C5-ACE076FB2EAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="106">
   <si>
     <t>TABLES</t>
   </si>
@@ -336,6 +336,15 @@
   </si>
   <si>
     <t>Buildings</t>
+  </si>
+  <si>
+    <t>Student Username</t>
+  </si>
+  <si>
+    <t>TABLE(S)</t>
+  </si>
+  <si>
+    <t>lecture_id</t>
   </si>
 </sst>
 </file>
@@ -998,8 +1007,1013 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I10" s="9"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C30" s="9"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="C31" s="9"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" ht="48.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+    </row>
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+    </row>
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+    </row>
+    <row r="44" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+    </row>
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+    </row>
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+    </row>
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+    </row>
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+    </row>
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+    </row>
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="5"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A61:H61"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1044,21 +2058,21 @@
         <v>15</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>16</v>
+        <v>78</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="10" t="s">
         <v>19</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="I3" s="9"/>
     </row>
@@ -1092,1001 +2106,6 @@
     </row>
     <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="9"/>
-    </row>
-    <row r="7" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-    </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-    </row>
-    <row r="30" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C30" s="9"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="C31" s="9"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-    </row>
-    <row r="32" spans="1:9" ht="48.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-    </row>
-    <row r="33" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-    </row>
-    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-    </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-    </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-    </row>
-    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-    </row>
-    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-    </row>
-    <row r="40" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-    </row>
-    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-    </row>
-    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-    </row>
-    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-    </row>
-    <row r="44" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-    </row>
-    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-    </row>
-    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-    </row>
-    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-    </row>
-    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="10"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-    </row>
-    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-    </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="9"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-    </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="10"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-    </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-    </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="9"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="5"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A60" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B61" s="13"/>
-      <c r="C61" s="13"/>
-      <c r="D61" s="13"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="4"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A62" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="4"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A63" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
-      <c r="F65" s="4"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A61:H61"/>
-  </mergeCells>
-  <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I69"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
-    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="11" t="s">

</xml_diff>

<commit_message>
lecture,etude registry and schedule
</commit_message>
<xml_diff>
--- a/project-evaluation.xlsx
+++ b/project-evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furka\Desktop\dersler\database\gitproje\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F416ECF-9B06-4AF7-81C5-ACE076FB2EAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20810ED-F6F1-4690-AE3D-12187094E3EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -329,9 +329,6 @@
     <t>Bulma</t>
   </si>
   <si>
-    <t>TIME(0)</t>
-  </si>
-  <si>
     <t>DATETIME(0)</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>lecture_id</t>
+  </si>
+  <si>
+    <t>TIME</t>
   </si>
 </sst>
 </file>
@@ -870,7 +870,7 @@
     </row>
     <row r="7" spans="1:3" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1141,7 +1141,7 @@
         <v>28</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I7" s="9"/>
     </row>
@@ -1157,7 +1157,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="8" t="s">
@@ -1273,7 +1273,7 @@
         <v>93</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="8" t="s">
@@ -1295,7 +1295,7 @@
         <v>93</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I15" s="9"/>
     </row>
@@ -1439,14 +1439,14 @@
         <v>45</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>18</v>
@@ -2012,7 +2012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>

</xml_diff>